<commit_message>
Global constant for campign data and enemy generator + new function to convert static data into entite on scene.
</commit_message>
<xml_diff>
--- a/documentation/DigimonDataBase.xlsx
+++ b/documentation/DigimonDataBase.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matheqs\Desktop\Hus 'n' Hus Game Studio\DRogue Lite\DRoque-Lite\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BAE4FE6-CFE1-48C3-A038-630D01C3C94C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81F944B6-D73E-4752-8FD1-E04DE7837201}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4095" yWindow="1785" windowWidth="12225" windowHeight="6870" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -76,7 +76,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -98,8 +98,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -114,6 +121,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
   </fills>
@@ -141,12 +153,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -154,8 +167,12 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
+    <cellStyle name="Bom" xfId="3" builtinId="26"/>
     <cellStyle name="Neutro" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Ruim" xfId="1" builtinId="27"/>
@@ -439,7 +456,7 @@
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -483,182 +500,182 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
+    <row r="2" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="3">
         <v>6</v>
       </c>
-      <c r="D2" s="2">
-        <v>1</v>
-      </c>
-      <c r="E2" s="2">
-        <v>3</v>
-      </c>
-      <c r="F2" s="2">
+      <c r="D2" s="3">
+        <v>1</v>
+      </c>
+      <c r="E2" s="3">
+        <v>3</v>
+      </c>
+      <c r="F2" s="3">
         <v>5</v>
       </c>
-      <c r="G2" s="2">
+      <c r="G2" s="3">
         <v>2</v>
       </c>
-      <c r="H2" s="2">
-        <v>3</v>
-      </c>
-      <c r="I2" s="2">
+      <c r="H2" s="3">
+        <v>3</v>
+      </c>
+      <c r="I2" s="3">
         <f>SUM(C2:H2)</f>
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
-        <v>1</v>
-      </c>
-      <c r="B3" s="2" t="s">
+    <row r="3" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="3">
         <v>5</v>
       </c>
-      <c r="D3" s="2">
-        <v>3</v>
-      </c>
-      <c r="E3" s="2">
+      <c r="D3" s="3">
+        <v>3</v>
+      </c>
+      <c r="E3" s="3">
         <v>2</v>
       </c>
-      <c r="F3" s="2">
-        <v>3</v>
-      </c>
-      <c r="G3" s="2">
-        <v>3</v>
-      </c>
-      <c r="H3" s="2">
+      <c r="F3" s="3">
+        <v>3</v>
+      </c>
+      <c r="G3" s="3">
+        <v>3</v>
+      </c>
+      <c r="H3" s="3">
         <v>4</v>
       </c>
-      <c r="I3" s="2">
+      <c r="I3" s="3">
         <f t="shared" ref="I3:I7" si="0">SUM(C3:H3)</f>
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
+    <row r="4" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
         <v>2</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="3">
         <v>5</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="3">
         <v>4</v>
       </c>
-      <c r="E4" s="2">
-        <v>1</v>
-      </c>
-      <c r="F4" s="2">
+      <c r="E4" s="3">
+        <v>1</v>
+      </c>
+      <c r="F4" s="3">
         <v>4</v>
       </c>
-      <c r="G4" s="2">
-        <v>3</v>
-      </c>
-      <c r="H4" s="2">
-        <v>3</v>
-      </c>
-      <c r="I4" s="2">
+      <c r="G4" s="3">
+        <v>3</v>
+      </c>
+      <c r="H4" s="3">
+        <v>3</v>
+      </c>
+      <c r="I4" s="3">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
-        <v>3</v>
-      </c>
-      <c r="B5" s="2" t="s">
+    <row r="5" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
+        <v>3</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="3">
         <v>8</v>
       </c>
-      <c r="D5" s="2">
-        <v>1</v>
-      </c>
-      <c r="E5" s="2">
+      <c r="D5" s="3">
+        <v>1</v>
+      </c>
+      <c r="E5" s="3">
         <v>5</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F5" s="3">
         <v>2</v>
       </c>
-      <c r="G5" s="2">
-        <v>1</v>
-      </c>
-      <c r="H5" s="2">
-        <v>3</v>
-      </c>
-      <c r="I5" s="2">
+      <c r="G5" s="3">
+        <v>1</v>
+      </c>
+      <c r="H5" s="3">
+        <v>3</v>
+      </c>
+      <c r="I5" s="3">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
+    <row r="6" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
         <v>4</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="3">
         <v>2</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="3">
         <v>7</v>
       </c>
-      <c r="E6" s="2">
-        <v>3</v>
-      </c>
-      <c r="F6" s="2">
+      <c r="E6" s="3">
+        <v>3</v>
+      </c>
+      <c r="F6" s="3">
         <v>4</v>
       </c>
-      <c r="G6" s="2">
-        <v>3</v>
-      </c>
-      <c r="H6" s="2">
-        <v>1</v>
-      </c>
-      <c r="I6" s="2">
+      <c r="G6" s="3">
+        <v>3</v>
+      </c>
+      <c r="H6" s="3">
+        <v>1</v>
+      </c>
+      <c r="I6" s="3">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
+    <row r="7" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
         <v>5</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="3">
         <v>4</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="3">
         <v>5</v>
       </c>
-      <c r="E7" s="2">
-        <v>1</v>
-      </c>
-      <c r="F7" s="2">
+      <c r="E7" s="3">
+        <v>1</v>
+      </c>
+      <c r="F7" s="3">
         <v>6</v>
       </c>
-      <c r="G7" s="2">
-        <v>1</v>
-      </c>
-      <c r="H7" s="2">
-        <v>3</v>
-      </c>
-      <c r="I7" s="2">
+      <c r="G7" s="3">
+        <v>1</v>
+      </c>
+      <c r="H7" s="3">
+        <v>3</v>
+      </c>
+      <c r="I7" s="3">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>

</xml_diff>

<commit_message>
Evolution system implemented. No visual effects or evolution condition yet. Tested using an item that forces evolution.
</commit_message>
<xml_diff>
--- a/documentation/DigimonDataBase.xlsx
+++ b/documentation/DigimonDataBase.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matheqs\Desktop\Hus 'n' Hus Game Studio\DRogue Lite\DRoque-Lite\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81F944B6-D73E-4752-8FD1-E04DE7837201}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60B64974-2303-48B5-8DF9-905248D0B234}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4095" yWindow="1785" windowWidth="12225" windowHeight="6870" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>DigimonID</t>
   </si>
@@ -70,6 +70,9 @@
   </si>
   <si>
     <t>Betamon</t>
+  </si>
+  <si>
+    <t>Greymon</t>
   </si>
 </sst>
 </file>
@@ -453,10 +456,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:I186"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="J91" sqref="J91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -680,6 +683,926 @@
         <v>20</v>
       </c>
     </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" s="2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" s="2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" s="2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" s="2">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" s="2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" s="2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" s="2">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" s="2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" s="2">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" s="2">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" s="2">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" s="2">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" s="2">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" s="2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" s="2">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" s="2">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" s="2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" s="2">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" s="2">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" s="2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" s="2">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" s="2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" s="2">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" s="2">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" s="2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" s="2">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" s="2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" s="2">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" s="2">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" s="2">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" s="2">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" s="2">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" s="2">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" s="2">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" s="2">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61" s="2">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62" s="2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" s="2">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64" s="2">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" s="2">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" s="2">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" s="2">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" s="2">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" s="2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70" s="2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71" s="2">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72" s="2">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A73" s="2">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74" s="2">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75" s="2">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A76" s="2">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77" s="2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A78" s="2">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A79" s="2">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A80" s="2">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A81" s="2">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A82" s="2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A83" s="2">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A84" s="2">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A85" s="2">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A86" s="2">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A87" s="2">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A88" s="3">
+        <v>86</v>
+      </c>
+      <c r="B88" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C88" s="3">
+        <v>8</v>
+      </c>
+      <c r="D88" s="3">
+        <v>3</v>
+      </c>
+      <c r="E88" s="3">
+        <v>4</v>
+      </c>
+      <c r="F88" s="3">
+        <v>7</v>
+      </c>
+      <c r="G88" s="3">
+        <v>4</v>
+      </c>
+      <c r="H88" s="3">
+        <v>4</v>
+      </c>
+      <c r="I88" s="3">
+        <f>SUM(C88:H88)</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A89" s="2">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A90" s="2">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A91" s="2">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A92" s="2">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A93" s="2">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A94" s="2">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A95" s="2">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A96" s="2">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A97" s="2">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A98" s="2">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A99" s="2">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A100" s="2">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A101" s="2">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A102" s="2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A103" s="2">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A104" s="2">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A105" s="2">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A106" s="2">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A107" s="2">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A108" s="2">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A109" s="2">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A110" s="2">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A111" s="2">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A112" s="2">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A113" s="2">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A114" s="2">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A115" s="2">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A116" s="2">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A117" s="2">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A118" s="2">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A119" s="2">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A120" s="2">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A121" s="2">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A122" s="2">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A123" s="2">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A124" s="2">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A125" s="2">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A126" s="2">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A127" s="2">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A128" s="2">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A129" s="2">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A130" s="2">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A131" s="2">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A132" s="2">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A133" s="2">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A134" s="2">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A135" s="2">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A136" s="2">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A137" s="2">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A138" s="2">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A139" s="2">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A140" s="2">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A141" s="2">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A142" s="2">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A143" s="2">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A144" s="2">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A145" s="2">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A146" s="2">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A147" s="2">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A148" s="2">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A149" s="2">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A150" s="2">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A151" s="2">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A152" s="2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A153" s="2">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A154" s="2">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="155" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A155" s="2">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="156" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A156" s="2">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="157" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A157" s="2">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="158" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A158" s="2">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="159" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A159" s="2">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="160" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A160" s="2">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A161" s="2">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A162" s="2">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="163" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A163" s="2">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="164" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A164" s="2">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="165" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A165" s="2">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="166" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A166" s="2">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="167" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A167" s="2">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="168" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A168" s="2">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="169" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A169" s="2">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="170" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A170" s="2">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="171" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A171" s="2">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="172" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A172" s="2">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="173" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A173" s="2">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="174" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A174" s="2">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="175" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A175" s="2">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="176" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A176" s="2">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="177" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A177" s="2">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="178" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A178" s="2">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="179" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A179" s="2">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="180" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A180" s="2">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="181" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A181" s="2">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="182" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A182" s="2">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="183" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A183" s="2">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="184" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A184" s="2">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="185" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A185" s="2">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="186" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A186" s="2">
+        <v>184</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Some digimon evolutions for depuration + stun status effect
</commit_message>
<xml_diff>
--- a/documentation/DigimonDataBase.xlsx
+++ b/documentation/DigimonDataBase.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matheqs\Desktop\Hus 'n' Hus Game Studio\DRogue Lite\DRoque-Lite\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60B64974-2303-48B5-8DF9-905248D0B234}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E402188-1C6D-478E-B935-4F219FBEDF18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>DigimonID</t>
   </si>
@@ -73,13 +73,22 @@
   </si>
   <si>
     <t>Greymon</t>
+  </si>
+  <si>
+    <t>Strikedramon</t>
+  </si>
+  <si>
+    <t>ExVeemon</t>
+  </si>
+  <si>
+    <t>Dorugamon</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -104,6 +113,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -162,7 +179,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -171,6 +188,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -458,8 +478,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I186"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="J91" sqref="J91"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E97" sqref="E97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1073,9 +1093,34 @@
         <v>83</v>
       </c>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A86" s="2">
+    <row r="86" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A86" s="3">
         <v>84</v>
+      </c>
+      <c r="B86" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C86" s="3">
+        <v>6</v>
+      </c>
+      <c r="D86" s="3">
+        <v>5</v>
+      </c>
+      <c r="E86" s="3">
+        <v>6</v>
+      </c>
+      <c r="F86" s="3">
+        <v>4</v>
+      </c>
+      <c r="G86" s="3">
+        <v>6</v>
+      </c>
+      <c r="H86" s="3">
+        <v>3</v>
+      </c>
+      <c r="I86" s="3">
+        <f t="shared" ref="I86" si="1">SUM(C86:H86)</f>
+        <v>30</v>
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.25">
@@ -1113,9 +1158,34 @@
         <v>30</v>
       </c>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A89" s="2">
+    <row r="89" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A89" s="3">
         <v>87</v>
+      </c>
+      <c r="B89" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C89" s="3">
+        <v>7</v>
+      </c>
+      <c r="D89" s="3">
+        <v>3</v>
+      </c>
+      <c r="E89" s="3">
+        <v>7</v>
+      </c>
+      <c r="F89" s="3">
+        <v>4</v>
+      </c>
+      <c r="G89" s="3">
+        <v>5</v>
+      </c>
+      <c r="H89" s="3">
+        <v>4</v>
+      </c>
+      <c r="I89" s="3">
+        <f t="shared" ref="I89" si="2">SUM(C89:H89)</f>
+        <v>30</v>
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.25">
@@ -1132,6 +1202,7 @@
       <c r="A92" s="2">
         <v>90</v>
       </c>
+      <c r="G92" s="4"/>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93" s="2">
@@ -1153,82 +1224,107 @@
         <v>94</v>
       </c>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97" s="2">
         <v>95</v>
       </c>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" s="2">
         <v>96</v>
       </c>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" s="2">
         <v>97</v>
       </c>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100" s="2">
         <v>98</v>
       </c>
     </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A101" s="2">
+    <row r="101" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A101" s="3">
         <v>99</v>
       </c>
-    </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B101" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C101" s="3">
+        <v>5</v>
+      </c>
+      <c r="D101" s="3">
+        <v>10</v>
+      </c>
+      <c r="E101" s="3">
+        <v>6</v>
+      </c>
+      <c r="F101" s="3">
+        <v>5</v>
+      </c>
+      <c r="G101" s="3">
+        <v>3</v>
+      </c>
+      <c r="H101" s="3">
+        <v>1</v>
+      </c>
+      <c r="I101" s="3">
+        <f t="shared" ref="I101" si="3">SUM(C101:H101)</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A102" s="2">
         <v>100</v>
       </c>
     </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A103" s="2">
         <v>101</v>
       </c>
     </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A104" s="2">
         <v>102</v>
       </c>
     </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A105" s="2">
         <v>103</v>
       </c>
     </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A106" s="2">
         <v>104</v>
       </c>
     </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A107" s="2">
         <v>105</v>
       </c>
     </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A108" s="2">
         <v>106</v>
       </c>
     </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A109" s="2">
         <v>107</v>
       </c>
     </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A110" s="2">
         <v>108</v>
       </c>
     </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A111" s="2">
         <v>109</v>
       </c>
     </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A112" s="2">
         <v>110</v>
       </c>

</xml_diff>

<commit_message>
Agi buuff and debuf plus Evolutuion teste and implementation
</commit_message>
<xml_diff>
--- a/documentation/DigimonDataBase.xlsx
+++ b/documentation/DigimonDataBase.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matheqs\Desktop\Hus 'n' Hus Game Studio\DRogue Lite\DRoque-Lite\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E402188-1C6D-478E-B935-4F219FBEDF18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{294B4F1E-82C7-46C3-94F9-1DD3C8F0D5B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>DigimonID</t>
   </si>
@@ -82,6 +82,12 @@
   </si>
   <si>
     <t>Dorugamon</t>
+  </si>
+  <si>
+    <t>Growlmon</t>
+  </si>
+  <si>
+    <t>Seadramon</t>
   </si>
 </sst>
 </file>
@@ -479,7 +485,7 @@
   <dimension ref="A1:I186"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E97" sqref="E97"/>
+      <selection activeCell="E71" sqref="E71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -988,82 +994,107 @@
         <v>62</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" s="2">
         <v>63</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" s="2">
         <v>64</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" s="2">
         <v>65</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A68" s="2">
+    <row r="68" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="3">
         <v>66</v>
       </c>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B68" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C68" s="3">
+        <v>5</v>
+      </c>
+      <c r="D68" s="3">
+        <v>8</v>
+      </c>
+      <c r="E68" s="3">
+        <v>5</v>
+      </c>
+      <c r="F68" s="3">
+        <v>6</v>
+      </c>
+      <c r="G68" s="3">
+        <v>3</v>
+      </c>
+      <c r="H68" s="3">
+        <v>3</v>
+      </c>
+      <c r="I68" s="3">
+        <f t="shared" ref="I68" si="1">SUM(C68:H68)</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" s="2">
         <v>67</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" s="2">
         <v>68</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" s="2">
         <v>69</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" s="2">
         <v>70</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" s="2">
         <v>71</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" s="2">
         <v>72</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" s="2">
         <v>73</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" s="2">
         <v>74</v>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" s="2">
         <v>75</v>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" s="2">
         <v>76</v>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" s="2">
         <v>77</v>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" s="2">
         <v>78</v>
       </c>
@@ -1119,7 +1150,7 @@
         <v>3</v>
       </c>
       <c r="I86" s="3">
-        <f t="shared" ref="I86" si="1">SUM(C86:H86)</f>
+        <f t="shared" ref="I86" si="2">SUM(C86:H86)</f>
         <v>30</v>
       </c>
     </row>
@@ -1184,7 +1215,7 @@
         <v>4</v>
       </c>
       <c r="I89" s="3">
-        <f t="shared" ref="I89" si="2">SUM(C89:H89)</f>
+        <f t="shared" ref="I89" si="3">SUM(C89:H89)</f>
         <v>30</v>
       </c>
     </row>
@@ -1193,9 +1224,34 @@
         <v>88</v>
       </c>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A91" s="2">
+    <row r="91" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A91" s="3">
         <v>89</v>
+      </c>
+      <c r="B91" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C91" s="3">
+        <v>9</v>
+      </c>
+      <c r="D91" s="3">
+        <v>7</v>
+      </c>
+      <c r="E91" s="3">
+        <v>6</v>
+      </c>
+      <c r="F91" s="3">
+        <v>3</v>
+      </c>
+      <c r="G91" s="3">
+        <v>2</v>
+      </c>
+      <c r="H91" s="3">
+        <v>3</v>
+      </c>
+      <c r="I91" s="3">
+        <f t="shared" ref="I91" si="4">SUM(C91:H91)</f>
+        <v>30</v>
       </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.25">
@@ -1270,7 +1326,7 @@
         <v>1</v>
       </c>
       <c r="I101" s="3">
-        <f t="shared" ref="I101" si="3">SUM(C101:H101)</f>
+        <f t="shared" ref="I101" si="5">SUM(C101:H101)</f>
         <v>30</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Wormmon Database addition and test
</commit_message>
<xml_diff>
--- a/documentation/DigimonDataBase.xlsx
+++ b/documentation/DigimonDataBase.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matheqs\Desktop\Hus 'n' Hus Game Studio\DRogue Lite\DRoque-Lite\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{294B4F1E-82C7-46C3-94F9-1DD3C8F0D5B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9979A409-5393-469A-8168-68CC49D664EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>DigimonID</t>
   </si>
@@ -88,6 +88,9 @@
   </si>
   <si>
     <t>Seadramon</t>
+  </si>
+  <si>
+    <t>Wormmon</t>
   </si>
 </sst>
 </file>
@@ -484,8 +487,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I186"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E71" sqref="E71"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21:XFD21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -754,82 +757,107 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" s="2">
+    <row r="21" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="3">
         <v>19</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B21" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C21" s="3">
+        <v>3</v>
+      </c>
+      <c r="D21" s="3">
+        <v>4</v>
+      </c>
+      <c r="E21" s="3">
+        <v>2</v>
+      </c>
+      <c r="F21" s="3">
+        <v>8</v>
+      </c>
+      <c r="G21" s="3">
+        <v>2</v>
+      </c>
+      <c r="H21" s="3">
+        <v>1</v>
+      </c>
+      <c r="I21" s="3">
+        <f t="shared" ref="I21" si="1">SUM(C21:H21)</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>30</v>
       </c>
@@ -1035,7 +1063,7 @@
         <v>3</v>
       </c>
       <c r="I68" s="3">
-        <f t="shared" ref="I68" si="1">SUM(C68:H68)</f>
+        <f t="shared" ref="I68" si="2">SUM(C68:H68)</f>
         <v>30</v>
       </c>
     </row>
@@ -1150,7 +1178,7 @@
         <v>3</v>
       </c>
       <c r="I86" s="3">
-        <f t="shared" ref="I86" si="2">SUM(C86:H86)</f>
+        <f t="shared" ref="I86" si="3">SUM(C86:H86)</f>
         <v>30</v>
       </c>
     </row>
@@ -1215,7 +1243,7 @@
         <v>4</v>
       </c>
       <c r="I89" s="3">
-        <f t="shared" ref="I89" si="3">SUM(C89:H89)</f>
+        <f t="shared" ref="I89" si="4">SUM(C89:H89)</f>
         <v>30</v>
       </c>
     </row>
@@ -1250,7 +1278,7 @@
         <v>3</v>
       </c>
       <c r="I91" s="3">
-        <f t="shared" ref="I91" si="4">SUM(C91:H91)</f>
+        <f t="shared" ref="I91" si="5">SUM(C91:H91)</f>
         <v>30</v>
       </c>
     </row>
@@ -1326,7 +1354,7 @@
         <v>1</v>
       </c>
       <c r="I101" s="3">
-        <f t="shared" ref="I101" si="5">SUM(C101:H101)</f>
+        <f t="shared" ref="I101" si="6">SUM(C101:H101)</f>
         <v>30</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Stingmon database and Wormmon evolution charts(setting teste scenario for fusion implementation)
</commit_message>
<xml_diff>
--- a/documentation/DigimonDataBase.xlsx
+++ b/documentation/DigimonDataBase.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matheqs\Desktop\Hus 'n' Hus Game Studio\DRogue Lite\DRoque-Lite\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9979A409-5393-469A-8168-68CC49D664EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2002617C-C42F-46FB-85E1-6C41AB9FA00A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,12 +20,23 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>DigimonID</t>
   </si>
@@ -91,6 +102,9 @@
   </si>
   <si>
     <t>Wormmon</t>
+  </si>
+  <si>
+    <t>Stingmon</t>
   </si>
 </sst>
 </file>
@@ -487,8 +501,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I186"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21:XFD21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H92" sqref="H92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1178,13 +1192,38 @@
         <v>3</v>
       </c>
       <c r="I86" s="3">
-        <f t="shared" ref="I86" si="3">SUM(C86:H86)</f>
+        <f t="shared" ref="I86:I87" si="3">SUM(C86:H86)</f>
         <v>30</v>
       </c>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A87" s="2">
+    <row r="87" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A87" s="3">
         <v>85</v>
+      </c>
+      <c r="B87" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C87" s="3">
+        <v>6</v>
+      </c>
+      <c r="D87" s="3">
+        <v>4</v>
+      </c>
+      <c r="E87" s="3">
+        <v>8</v>
+      </c>
+      <c r="F87" s="3">
+        <v>8</v>
+      </c>
+      <c r="G87" s="3">
+        <v>3</v>
+      </c>
+      <c r="H87" s="3">
+        <v>1</v>
+      </c>
+      <c r="I87" s="3">
+        <f t="shared" si="3"/>
+        <v>30</v>
       </c>
     </row>
     <row r="88" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Digimon Ultimate Tier test
</commit_message>
<xml_diff>
--- a/documentation/DigimonDataBase.xlsx
+++ b/documentation/DigimonDataBase.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matheqs\Desktop\Hus 'n' Hus Game Studio\DRogue Lite\DRoque-Lite\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2002617C-C42F-46FB-85E1-6C41AB9FA00A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13A9DCB4-13FF-486F-B252-DBA816875275}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,23 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>DigimonID</t>
   </si>
@@ -105,6 +94,9 @@
   </si>
   <si>
     <t>Stingmon</t>
+  </si>
+  <si>
+    <t>Paildramon</t>
   </si>
 </sst>
 </file>
@@ -499,10 +491,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I186"/>
+  <dimension ref="A1:I279"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H92" sqref="H92"/>
+    <sheetView tabSelected="1" topLeftCell="A187" workbookViewId="0">
+      <selection activeCell="A202" sqref="A202:XFD202"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1822,6 +1814,496 @@
         <v>184</v>
       </c>
     </row>
+    <row r="187" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A187" s="2">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="188" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A188" s="2">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="189" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A189" s="2">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="190" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A190" s="2">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="191" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A191" s="2">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="192" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A192" s="2">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="193" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A193" s="2">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="194" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A194" s="2">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="195" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A195" s="2">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="196" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A196" s="2">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="197" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A197" s="2">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="198" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A198" s="2">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="199" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A199" s="2">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="200" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A200" s="2">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="201" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A201" s="2">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="202" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A202" s="3">
+        <v>200</v>
+      </c>
+      <c r="B202" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C202" s="3">
+        <v>8</v>
+      </c>
+      <c r="D202" s="3">
+        <v>11</v>
+      </c>
+      <c r="E202" s="3">
+        <v>7</v>
+      </c>
+      <c r="F202" s="3">
+        <v>9</v>
+      </c>
+      <c r="G202" s="3">
+        <v>3</v>
+      </c>
+      <c r="H202" s="3">
+        <v>2</v>
+      </c>
+      <c r="I202" s="3">
+        <f t="shared" ref="I202" si="7">SUM(C202:H202)</f>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="203" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A203" s="2">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="204" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A204" s="2">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="205" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A205" s="2">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="206" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A206" s="2">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="207" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A207" s="2">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="208" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A208" s="2">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="209" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A209" s="2">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="210" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A210" s="2">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="211" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A211" s="2">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="212" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A212" s="2">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="213" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A213" s="2">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="214" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A214" s="2">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="215" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A215" s="2">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="216" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A216" s="2">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="217" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A217" s="2">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="218" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A218" s="2">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="219" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A219" s="2">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="220" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A220" s="2">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="221" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A221" s="2">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="222" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A222" s="2">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="223" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A223" s="2">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="224" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A224" s="2">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="225" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A225" s="2">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="226" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A226" s="2">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="227" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A227" s="2">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="228" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A228" s="2">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="229" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A229" s="2">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="230" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A230" s="2">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="231" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A231" s="2">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="232" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A232" s="2">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="233" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A233" s="2">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="234" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A234" s="2">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="235" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A235" s="2">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="236" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A236" s="2">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="237" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A237" s="2">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="238" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A238" s="2">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="239" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A239" s="2">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="240" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A240" s="2">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="241" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A241" s="2">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="242" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A242" s="2">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="243" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A243" s="2">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="244" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A244" s="2">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="245" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A245" s="2">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="246" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A246" s="2">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="247" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A247" s="2">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="248" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A248" s="2">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="249" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A249" s="2">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="250" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A250" s="2">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="251" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A251" s="2">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="252" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A252" s="2">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="253" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A253" s="2">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="254" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A254" s="2">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="255" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A255" s="2">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="256" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A256" s="2">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="257" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A257" s="2">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="258" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A258" s="2">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="259" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A259" s="2">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="260" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A260" s="2">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="261" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A261" s="2">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="262" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A262" s="2">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="263" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A263" s="2">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="264" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A264" s="2">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="265" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A265" s="2">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="266" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A266" s="2">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="267" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A267" s="2">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="268" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A268" s="2">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="269" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A269" s="2">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="270" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A270" s="2">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="271" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A271" s="2">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="272" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A272" s="2">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="273" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A273" s="2">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="274" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A274" s="2">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="275" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A275" s="2">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="276" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A276" s="2">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="277" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A277" s="2">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="278" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A278" s="2">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="279" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A279" s="2">
+        <v>277</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>